<commit_message>
Modify full search method
</commit_message>
<xml_diff>
--- a/output/exchange_rate.xlsx
+++ b/output/exchange_rate.xlsx
@@ -378,7 +378,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="n">
-        <v>108.8127389529253</v>
+        <v>106.9156030070433</v>
       </c>
       <c r="B1" s="0" t="n">
         <v>108.8127389529253</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="n">
-        <v>108.8127389529253</v>
+        <v>106.9156030070433</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>106.9156030070433</v>
@@ -1284,7 +1284,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="n">
-        <v>109.7738935512468</v>
+        <v>105.9794749338002</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>107.86</v>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="5">
       <c r="A5" s="0" t="n">
-        <v>108.8127389529254</v>
+        <v>105.051543379539</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>108.8127389529254</v>
@@ -1888,7 +1888,7 @@
     </row>
     <row r="6">
       <c r="A6" s="0" t="n">
-        <v>107.86</v>
+        <v>105.9794749338002</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>109.7738935512468</v>
@@ -2190,7 +2190,7 @@
     </row>
     <row r="7">
       <c r="A7" s="0" t="n">
-        <v>108.8127389529254</v>
+        <v>106.9156030070433</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>110.743538131263</v>
@@ -2492,7 +2492,7 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="n">
-        <v>109.7738935512468</v>
+        <v>105.9794749338002</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>111.7217476858933</v>
@@ -2794,7 +2794,7 @@
     </row>
     <row r="9">
       <c r="A9" s="0" t="n">
-        <v>110.743538131263</v>
+        <v>106.9156030070434</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>112.7085978704775</v>
@@ -3096,7 +3096,7 @@
     </row>
     <row r="10">
       <c r="A10" s="0" t="n">
-        <v>109.7738935512468</v>
+        <v>105.9794749338002</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>111.7217476858934</v>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="11">
       <c r="A11" s="0" t="n">
-        <v>110.7435381312631</v>
+        <v>105.0515433795391</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>112.7085978704775</v>
@@ -3700,7 +3700,7 @@
     </row>
     <row r="12">
       <c r="A12" s="0" t="n">
-        <v>109.7738935512468</v>
+        <v>105.9794749338002</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>113.704165008627</v>
@@ -4002,7 +4002,7 @@
     </row>
     <row r="13">
       <c r="A13" s="0" t="n">
-        <v>108.8127389529254</v>
+        <v>106.9156030070434</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>112.7085978704775</v>
@@ -4304,7 +4304,7 @@
     </row>
     <row r="14">
       <c r="A14" s="0" t="n">
-        <v>109.7738935512469</v>
+        <v>105.9794749338003</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>113.704165008627</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="15">
       <c r="A15" s="0" t="n">
-        <v>108.8127389529255</v>
+        <v>106.9156030070434</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>114.7085260981279</v>
@@ -5210,7 +5210,7 @@
     </row>
     <row r="17">
       <c r="A17" s="0" t="n">
-        <v>106.9156030070434</v>
+        <v>108.8127389529254</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>116.7439415289848</v>
@@ -5512,7 +5512,7 @@
     </row>
     <row r="18">
       <c r="A18" s="0" t="n">
-        <v>105.9794749338003</v>
+        <v>109.7738935512469</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>117.7751532906453</v>
@@ -5814,7 +5814,7 @@
     </row>
     <row r="19">
       <c r="A19" s="0" t="n">
-        <v>105.0515433795391</v>
+        <v>110.7435381312631</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>116.7439415289849</v>
@@ -6116,7 +6116,7 @@
     </row>
     <row r="20">
       <c r="A20" s="0" t="n">
-        <v>104.1317365774522</v>
+        <v>111.7217476858934</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>115.7217588168962</v>
@@ -6418,7 +6418,7 @@
     </row>
     <row r="21">
       <c r="A21" s="0" t="n">
-        <v>103.2199833891052</v>
+        <v>112.7085978704776</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>114.708526098128</v>
@@ -6720,7 +6720,7 @@
     </row>
     <row r="22">
       <c r="A22" s="0" t="n">
-        <v>102.3162132989355</v>
+        <v>111.7217476858935</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>115.7217588168962</v>
@@ -7022,7 +7022,7 @@
     </row>
     <row r="23">
       <c r="A23" s="0" t="n">
-        <v>101.420356408798</v>
+        <v>110.7435381312632</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>114.708526098128</v>
@@ -7324,7 +7324,7 @@
     </row>
     <row r="24">
       <c r="A24" s="0" t="n">
-        <v>102.3162132989355</v>
+        <v>109.7738935512469</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>115.7217588168962</v>
@@ -7626,7 +7626,7 @@
     </row>
     <row r="25">
       <c r="A25" s="0" t="n">
-        <v>101.420356408798</v>
+        <v>108.8127389529255</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>114.708526098128</v>
@@ -7928,7 +7928,7 @@
     </row>
     <row r="26">
       <c r="A26" s="0" t="n">
-        <v>102.3162132989355</v>
+        <v>107.8600000000002</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>115.7217588168962</v>
@@ -8230,7 +8230,7 @@
     </row>
     <row r="27">
       <c r="A27" s="0" t="n">
-        <v>103.2199833891053</v>
+        <v>106.9156030070435</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>116.7439415289849</v>
@@ -8532,7 +8532,7 @@
     </row>
     <row r="28">
       <c r="A28" s="0" t="n">
-        <v>102.3162132989355</v>
+        <v>105.9794749338004</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>115.7217588168962</v>
@@ -8834,7 +8834,7 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="n">
-        <v>101.420356408798</v>
+        <v>105.0515433795392</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>116.7439415289849</v>
@@ -9136,7 +9136,7 @@
     </row>
     <row r="30">
       <c r="A30" s="0" t="n">
-        <v>100.5323434325597</v>
+        <v>105.9794749338004</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>117.7751532906454</v>
@@ -9438,7 +9438,7 @@
     </row>
     <row r="31">
       <c r="A31" s="0" t="n">
-        <v>99.6521056907407</v>
+        <v>106.9156030070436</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>116.7439415289849</v>
@@ -9740,7 +9740,7 @@
     </row>
     <row r="32">
       <c r="A32" s="0" t="n">
-        <v>100.5323434325597</v>
+        <v>107.8600000000003</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>117.7751532906454</v>
@@ -10042,7 +10042,7 @@
     </row>
     <row r="33">
       <c r="A33" s="0" t="n">
-        <v>101.4203564087981</v>
+        <v>108.8127389529256</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>116.743941528985</v>
@@ -10344,7 +10344,7 @@
     </row>
     <row r="34">
       <c r="A34" s="0" t="n">
-        <v>100.5323434325597</v>
+        <v>109.773893551247</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>115.7217588168963</v>
@@ -10646,7 +10646,7 @@
     </row>
     <row r="35">
       <c r="A35" s="0" t="n">
-        <v>101.4203564087981</v>
+        <v>110.7435381312633</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>116.743941528985</v>
@@ -10948,7 +10948,7 @@
     </row>
     <row r="36">
       <c r="A36" s="0" t="n">
-        <v>100.5323434325598</v>
+        <v>111.7217476858936</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>115.7217588168963</v>
@@ -11250,7 +11250,7 @@
     </row>
     <row r="37">
       <c r="A37" s="0" t="n">
-        <v>99.65210569074074</v>
+        <v>112.7085978704778</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>114.7085260981281</v>
@@ -11552,7 +11552,7 @@
     </row>
     <row r="38">
       <c r="A38" s="0" t="n">
-        <v>100.5323434325598</v>
+        <v>111.7217476858936</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>115.7217588168963</v>
@@ -11854,7 +11854,7 @@
     </row>
     <row r="39">
       <c r="A39" s="0" t="n">
-        <v>101.4203564087981</v>
+        <v>112.7085978704778</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>116.743941528985</v>
@@ -12156,7 +12156,7 @@
     </row>
     <row r="40">
       <c r="A40" s="0" t="n">
-        <v>102.3162132989356</v>
+        <v>113.7041650086272</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>115.7217588168963</v>
@@ -12458,7 +12458,7 @@
     </row>
     <row r="41">
       <c r="A41" s="0" t="n">
-        <v>101.4203564087981</v>
+        <v>112.7085978704778</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>114.7085260981281</v>
@@ -12760,7 +12760,7 @@
     </row>
     <row r="42">
       <c r="A42" s="0" t="n">
-        <v>100.5323434325598</v>
+        <v>111.7217476858936</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>113.7041650086272</v>
@@ -13062,7 +13062,7 @@
     </row>
     <row r="43">
       <c r="A43" s="0" t="n">
-        <v>101.4203564087982</v>
+        <v>110.7435381312633</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>114.7085260981281</v>
@@ -13364,7 +13364,7 @@
     </row>
     <row r="44">
       <c r="A44" s="0" t="n">
-        <v>102.3162132989357</v>
+        <v>109.7738935512471</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>115.7217588168963</v>
@@ -13666,7 +13666,7 @@
     </row>
     <row r="45">
       <c r="A45" s="0" t="n">
-        <v>101.4203564087982</v>
+        <v>108.8127389529257</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>116.743941528985</v>
@@ -13968,7 +13968,7 @@
     </row>
     <row r="46">
       <c r="A46" s="0" t="n">
-        <v>100.5323434325598</v>
+        <v>107.8600000000004</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>115.7217588168964</v>
@@ -14270,7 +14270,7 @@
     </row>
     <row r="47">
       <c r="A47" s="0" t="n">
-        <v>101.4203564087982</v>
+        <v>108.8127389529257</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>116.7439415289851</v>
@@ -14572,7 +14572,7 @@
     </row>
     <row r="48">
       <c r="A48" s="0" t="n">
-        <v>100.5323434325599</v>
+        <v>107.8600000000004</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>115.7217588168964</v>
@@ -14874,7 +14874,7 @@
     </row>
     <row r="49">
       <c r="A49" s="0" t="n">
-        <v>101.4203564087982</v>
+        <v>106.9156030070437</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>114.7085260981282</v>
@@ -15176,7 +15176,7 @@
     </row>
     <row r="50">
       <c r="A50" s="0" t="n">
-        <v>100.5323434325599</v>
+        <v>105.9794749338006</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>115.7217588168964</v>
@@ -15478,7 +15478,7 @@
     </row>
     <row r="51">
       <c r="A51" s="0" t="n">
-        <v>101.4203564087982</v>
+        <v>105.0515433795394</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>116.7439415289851</v>
@@ -15780,7 +15780,7 @@
     </row>
     <row r="52">
       <c r="A52" s="0" t="n">
-        <v>102.3162132989357</v>
+        <v>104.1317365774525</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>115.7217588168964</v>
@@ -16082,7 +16082,7 @@
     </row>
     <row r="53">
       <c r="A53" s="0" t="n">
-        <v>101.4203564087982</v>
+        <v>105.0515433795394</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>116.7439415289851</v>
@@ -16384,7 +16384,7 @@
     </row>
     <row r="54">
       <c r="A54" s="0" t="n">
-        <v>102.3162132989358</v>
+        <v>105.9794749338006</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>117.7751532906456</v>
@@ -16686,7 +16686,7 @@
     </row>
     <row r="55">
       <c r="A55" s="0" t="n">
-        <v>103.2199833891055</v>
+        <v>106.9156030070438</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>118.8154738564415</v>
@@ -16988,7 +16988,7 @@
     </row>
     <row r="56">
       <c r="A56" s="0" t="n">
-        <v>102.3162132989358</v>
+        <v>107.8600000000005</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>119.8649836854172</v>
@@ -17290,7 +17290,7 @@
     </row>
     <row r="57">
       <c r="A57" s="0" t="n">
-        <v>103.2199833891056</v>
+        <v>106.9156030070438</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>120.9237639473202</v>
@@ -17592,7 +17592,7 @@
     </row>
     <row r="58">
       <c r="A58" s="0" t="n">
-        <v>104.1317365774525</v>
+        <v>105.9794749338007</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>121.9918965288792</v>
@@ -17894,7 +17894,7 @@
     </row>
     <row r="59">
       <c r="A59" s="0" t="n">
-        <v>103.2199833891056</v>
+        <v>106.9156030070438</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>120.9237639473202</v>
@@ -18196,7 +18196,7 @@
     </row>
     <row r="60">
       <c r="A60" s="0" t="n">
-        <v>102.3162132989358</v>
+        <v>107.8600000000006</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>119.8649836854172</v>
@@ -18498,7 +18498,7 @@
     </row>
     <row r="61">
       <c r="A61" s="0" t="n">
-        <v>101.4203564087983</v>
+        <v>108.8127389529259</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>118.8154738564416</v>
@@ -18800,7 +18800,7 @@
     </row>
     <row r="62">
       <c r="A62" s="0" t="n">
-        <v>100.53234343256</v>
+        <v>107.8600000000006</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>117.7751532906457</v>
@@ -19102,7 +19102,7 @@
     </row>
     <row r="63">
       <c r="A63" s="0" t="n">
-        <v>99.65210569074094</v>
+        <v>106.9156030070439</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>116.7439415289852</v>
@@ -19404,7 +19404,7 @@
     </row>
     <row r="64">
       <c r="A64" s="0" t="n">
-        <v>98.77957510520285</v>
+        <v>107.8600000000006</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>117.7751532906457</v>
@@ -19706,7 +19706,7 @@
     </row>
     <row r="65">
       <c r="A65" s="0" t="n">
-        <v>97.9146841938836</v>
+        <v>106.9156030070439</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>116.7439415289852</v>
@@ -20008,7 +20008,7 @@
     </row>
     <row r="66">
       <c r="A66" s="0" t="n">
-        <v>97.05736606557831</v>
+        <v>105.9794749338008</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>115.7217588168965</v>
@@ -20310,7 +20310,7 @@
     </row>
     <row r="67">
       <c r="A67" s="0" t="n">
-        <v>96.20755441476587</v>
+        <v>105.0515433795396</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>114.7085260981283</v>
@@ -20612,7 +20612,7 @@
     </row>
     <row r="68">
       <c r="A68" s="0" t="n">
-        <v>95.36518351648084</v>
+        <v>104.1317365774527</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>113.7041650086274</v>
@@ -20914,7 +20914,7 @@
     </row>
     <row r="69">
       <c r="A69" s="0" t="n">
-        <v>96.20755441476588</v>
+        <v>103.2199833891057</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>112.708597870478</v>
@@ -21216,7 +21216,7 @@
     </row>
     <row r="70">
       <c r="A70" s="0" t="n">
-        <v>95.36518351648085</v>
+        <v>104.1317365774527</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>111.7217476858938</v>
@@ -21518,7 +21518,7 @@
     </row>
     <row r="71">
       <c r="A71" s="0" t="n">
-        <v>94.53018822123028</v>
+        <v>103.2199833891057</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>112.708597870478</v>
@@ -21820,7 +21820,7 @@
     </row>
     <row r="72">
       <c r="A72" s="0" t="n">
-        <v>95.36518351648088</v>
+        <v>102.3162132989359</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>111.7217476858938</v>
@@ -22122,7 +22122,7 @@
     </row>
     <row r="73">
       <c r="A73" s="0" t="n">
-        <v>94.5301882212303</v>
+        <v>101.4203564087984</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>112.708597870478</v>
@@ -22424,7 +22424,7 @@
     </row>
     <row r="74">
       <c r="A74" s="0" t="n">
-        <v>93.70250394995495</v>
+        <v>102.3162132989359</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>113.7041650086275</v>
@@ -22726,7 +22726,7 @@
     </row>
     <row r="75">
       <c r="A75" s="0" t="n">
-        <v>94.53018822123032</v>
+        <v>101.4203564087984</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>114.7085260981284</v>
@@ -23028,7 +23028,7 @@
     </row>
     <row r="76">
       <c r="A76" s="0" t="n">
-        <v>93.70250394995496</v>
+        <v>100.5323434325601</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>115.7217588168966</v>
@@ -23330,7 +23330,7 @@
     </row>
     <row r="77">
       <c r="A77" s="0" t="n">
-        <v>92.88206668903479</v>
+        <v>101.4203564087984</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>116.7439415289853</v>
@@ -23632,7 +23632,7 @@
     </row>
     <row r="78">
       <c r="A78" s="0" t="n">
-        <v>92.06881298533807</v>
+        <v>100.5323434325601</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>117.7751532906458</v>
@@ -23934,7 +23934,7 @@
     </row>
     <row r="79">
       <c r="A79" s="0" t="n">
-        <v>91.26267994131391</v>
+        <v>101.4203564087985</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>116.7439415289853</v>
@@ -24236,7 +24236,7 @@
     </row>
     <row r="80">
       <c r="A80" s="0" t="n">
-        <v>92.06881298533808</v>
+        <v>102.316213298936</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>117.7751532906458</v>
@@ -24538,7 +24538,7 @@
     </row>
     <row r="81">
       <c r="A81" s="0" t="n">
-        <v>91.26267994131392</v>
+        <v>101.4203564087985</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>116.7439415289853</v>
@@ -24840,7 +24840,7 @@
     </row>
     <row r="82">
       <c r="A82" s="0" t="n">
-        <v>90.4636052101277</v>
+        <v>102.316213298936</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>115.7217588168966</v>
@@ -25142,7 +25142,7 @@
     </row>
     <row r="83">
       <c r="A83" s="0" t="n">
-        <v>89.67152699083911</v>
+        <v>103.2199833891058</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>116.7439415289853</v>
@@ -25444,7 +25444,7 @@
     </row>
     <row r="84">
       <c r="A84" s="0" t="n">
-        <v>88.8863840236225</v>
+        <v>104.1317365774528</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>117.7751532906458</v>
@@ -25746,7 +25746,7 @@
     </row>
     <row r="85">
       <c r="A85" s="0" t="n">
-        <v>89.67152699083913</v>
+        <v>105.0515433795397</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>116.7439415289853</v>
@@ -26048,7 +26048,7 @@
     </row>
     <row r="86">
       <c r="A86" s="0" t="n">
-        <v>88.88638402362251</v>
+        <v>105.9794749338009</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>117.7751532906458</v>
@@ -26350,7 +26350,7 @@
     </row>
     <row r="87">
       <c r="A87" s="0" t="n">
-        <v>89.67152699083914</v>
+        <v>106.9156030070441</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>116.7439415289854</v>
@@ -26652,7 +26652,7 @@
     </row>
     <row r="88">
       <c r="A88" s="0" t="n">
-        <v>88.88638402362253</v>
+        <v>105.9794749338009</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>117.7751532906459</v>
@@ -26954,7 +26954,7 @@
     </row>
     <row r="89">
       <c r="A89" s="0" t="n">
-        <v>89.67152699083915</v>
+        <v>106.9156030070441</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>116.7439415289854</v>
@@ -27256,7 +27256,7 @@
     </row>
     <row r="90">
       <c r="A90" s="0" t="n">
-        <v>88.88638402362254</v>
+        <v>107.8600000000008</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>115.7217588168967</v>
@@ -27558,7 +27558,7 @@
     </row>
     <row r="91">
       <c r="A91" s="0" t="n">
-        <v>89.67152699083917</v>
+        <v>106.9156030070441</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>116.7439415289854</v>
@@ -27860,7 +27860,7 @@
     </row>
     <row r="92">
       <c r="A92" s="0" t="n">
-        <v>90.46360521012777</v>
+        <v>105.979474933801</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>115.7217588168967</v>
@@ -28162,7 +28162,7 @@
     </row>
     <row r="93">
       <c r="A93" s="0" t="n">
-        <v>89.67152699083918</v>
+        <v>106.9156030070441</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>116.7439415289854</v>
@@ -28464,7 +28464,7 @@
     </row>
     <row r="94">
       <c r="A94" s="0" t="n">
-        <v>88.88638402362257</v>
+        <v>107.8600000000009</v>
       </c>
       <c r="B94" s="0" t="n">
         <v>115.7217588168967</v>
@@ -28766,7 +28766,7 @@
     </row>
     <row r="95">
       <c r="A95" s="0" t="n">
-        <v>89.6715269908392</v>
+        <v>108.8127389529262</v>
       </c>
       <c r="B95" s="0" t="n">
         <v>114.7085260981285</v>
@@ -29068,7 +29068,7 @@
     </row>
     <row r="96">
       <c r="A96" s="0" t="n">
-        <v>90.4636052101278</v>
+        <v>109.7738935512476</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>113.7041650086276</v>
@@ -29370,7 +29370,7 @@
     </row>
     <row r="97">
       <c r="A97" s="0" t="n">
-        <v>89.67152699083921</v>
+        <v>110.7435381312639</v>
       </c>
       <c r="B97" s="0" t="n">
         <v>112.7085978704782</v>
@@ -29672,7 +29672,7 @@
     </row>
     <row r="98">
       <c r="A98" s="0" t="n">
-        <v>90.46360521012781</v>
+        <v>111.7217476858942</v>
       </c>
       <c r="B98" s="0" t="n">
         <v>113.7041650086276</v>
@@ -29974,7 +29974,7 @@
     </row>
     <row r="99">
       <c r="A99" s="0" t="n">
-        <v>91.26267994131405</v>
+        <v>110.7435381312639</v>
       </c>
       <c r="B99" s="0" t="n">
         <v>112.7085978704782</v>
@@ -30276,7 +30276,7 @@
     </row>
     <row r="100">
       <c r="A100" s="0" t="n">
-        <v>90.46360521012782</v>
+        <v>111.7217476858942</v>
       </c>
       <c r="B100" s="0" t="n">
         <v>113.7041650086276</v>
@@ -30578,7 +30578,7 @@
     </row>
     <row r="101">
       <c r="A101" s="0" t="n">
-        <v>91.26267994131406</v>
+        <v>112.7085978704784</v>
       </c>
       <c r="B101" s="0" t="n">
         <v>114.7085260981286</v>
@@ -30880,7 +30880,7 @@
     </row>
     <row r="102">
       <c r="A102" s="0" t="n">
-        <v>90.46360521012784</v>
+        <v>111.7217476858942</v>
       </c>
       <c r="B102" s="0" t="n">
         <v>115.7217588168968</v>
@@ -31182,7 +31182,7 @@
     </row>
     <row r="103">
       <c r="A103" s="0" t="n">
-        <v>91.26267994131408</v>
+        <v>112.7085978704784</v>
       </c>
       <c r="B103" s="0" t="n">
         <v>114.7085260981286</v>
@@ -31484,7 +31484,7 @@
     </row>
     <row r="104">
       <c r="A104" s="0" t="n">
-        <v>92.06881298533825</v>
+        <v>113.7041650086279</v>
       </c>
       <c r="B104" s="0" t="n">
         <v>113.7041650086277</v>
@@ -31786,7 +31786,7 @@
     </row>
     <row r="105">
       <c r="A105" s="0" t="n">
-        <v>92.88206668903499</v>
+        <v>112.7085978704784</v>
       </c>
       <c r="B105" s="0" t="n">
         <v>114.7085260981286</v>
@@ -32088,7 +32088,7 @@
     </row>
     <row r="106">
       <c r="A106" s="0" t="n">
-        <v>92.06881298533827</v>
+        <v>111.7217476858943</v>
       </c>
       <c r="B106" s="0" t="n">
         <v>115.7217588168968</v>
@@ -32390,7 +32390,7 @@
     </row>
     <row r="107">
       <c r="A107" s="0" t="n">
-        <v>92.882066689035</v>
+        <v>110.7435381312639</v>
       </c>
       <c r="B107" s="0" t="n">
         <v>116.7439415289855</v>
@@ -32692,7 +32692,7 @@
     </row>
     <row r="108">
       <c r="A108" s="0" t="n">
-        <v>92.06881298533828</v>
+        <v>109.7738935512477</v>
       </c>
       <c r="B108" s="0" t="n">
         <v>117.775153290646</v>
@@ -32994,7 +32994,7 @@
     </row>
     <row r="109">
       <c r="A109" s="0" t="n">
-        <v>92.88206668903501</v>
+        <v>110.743538131264</v>
       </c>
       <c r="B109" s="0" t="n">
         <v>116.7439415289855</v>
@@ -33296,7 +33296,7 @@
     </row>
     <row r="110">
       <c r="A110" s="0" t="n">
-        <v>92.0688129853383</v>
+        <v>109.7738935512477</v>
       </c>
       <c r="B110" s="0" t="n">
         <v>115.7217588168968</v>
@@ -33598,7 +33598,7 @@
     </row>
     <row r="111">
       <c r="A111" s="0" t="n">
-        <v>91.26267994131413</v>
+        <v>110.743538131264</v>
       </c>
       <c r="B111" s="0" t="n">
         <v>114.7085260981286</v>
@@ -33900,7 +33900,7 @@
     </row>
     <row r="112">
       <c r="A112" s="0" t="n">
-        <v>92.06881298533831</v>
+        <v>111.7217476858943</v>
       </c>
       <c r="B112" s="0" t="n">
         <v>115.7217588168968</v>
@@ -34202,7 +34202,7 @@
     </row>
     <row r="113">
       <c r="A113" s="0" t="n">
-        <v>92.88206668903504</v>
+        <v>110.743538131264</v>
       </c>
       <c r="B113" s="0" t="n">
         <v>114.7085260981286</v>
@@ -34504,7 +34504,7 @@
     </row>
     <row r="114">
       <c r="A114" s="0" t="n">
-        <v>93.70250394995524</v>
+        <v>109.7738935512478</v>
       </c>
       <c r="B114" s="0" t="n">
         <v>113.7041650086277</v>
@@ -34806,7 +34806,7 @@
     </row>
     <row r="115">
       <c r="A115" s="0" t="n">
-        <v>92.88206668903506</v>
+        <v>108.8127389529263</v>
       </c>
       <c r="B115" s="0" t="n">
         <v>114.7085260981287</v>
@@ -35108,7 +35108,7 @@
     </row>
     <row r="116">
       <c r="A116" s="0" t="n">
-        <v>92.06881298533834</v>
+        <v>109.7738935512478</v>
       </c>
       <c r="B116" s="0" t="n">
         <v>113.7041650086278</v>
@@ -35410,7 +35410,7 @@
     </row>
     <row r="117">
       <c r="A117" s="0" t="n">
-        <v>92.88206668903507</v>
+        <v>108.8127389529264</v>
       </c>
       <c r="B117" s="0" t="n">
         <v>114.7085260981287</v>
@@ -35712,7 +35712,7 @@
     </row>
     <row r="118">
       <c r="A118" s="0" t="n">
-        <v>92.06881298533835</v>
+        <v>109.7738935512478</v>
       </c>
       <c r="B118" s="0" t="n">
         <v>113.7041650086278</v>
@@ -36014,7 +36014,7 @@
     </row>
     <row r="119">
       <c r="A119" s="0" t="n">
-        <v>92.88206668903509</v>
+        <v>110.743538131264</v>
       </c>
       <c r="B119" s="0" t="n">
         <v>112.7085978704783</v>
@@ -36316,7 +36316,7 @@
     </row>
     <row r="120">
       <c r="A120" s="0" t="n">
-        <v>93.70250394995529</v>
+        <v>111.7217476858944</v>
       </c>
       <c r="B120" s="0" t="n">
         <v>113.7041650086278</v>
@@ -36618,7 +36618,7 @@
     </row>
     <row r="121">
       <c r="A121" s="0" t="n">
-        <v>92.8820666890351</v>
+        <v>110.743538131264</v>
       </c>
       <c r="B121" s="0" t="n">
         <v>114.7085260981287</v>
@@ -36920,7 +36920,7 @@
     </row>
     <row r="122">
       <c r="A122" s="0" t="n">
-        <v>92.06881298533838</v>
+        <v>111.7217476858944</v>
       </c>
       <c r="B122" s="0" t="n">
         <v>113.7041650086278</v>
@@ -37222,7 +37222,7 @@
     </row>
     <row r="123">
       <c r="A123" s="0" t="n">
-        <v>92.88206668903511</v>
+        <v>112.7085978704785</v>
       </c>
       <c r="B123" s="0" t="n">
         <v>114.7085260981287</v>
@@ -37524,7 +37524,7 @@
     </row>
     <row r="124">
       <c r="A124" s="0" t="n">
-        <v>93.70250394995531</v>
+        <v>113.704165008628</v>
       </c>
       <c r="B124" s="0" t="n">
         <v>113.7041650086278</v>
@@ -37826,7 +37826,7 @@
     </row>
     <row r="125">
       <c r="A125" s="0" t="n">
-        <v>94.5301882212307</v>
+        <v>112.7085978704786</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>112.7085978704784</v>
@@ -38128,7 +38128,7 @@
     </row>
     <row r="126">
       <c r="A126" s="0" t="n">
-        <v>95.36518351648131</v>
+        <v>113.704165008628</v>
       </c>
       <c r="B126" s="0" t="n">
         <v>111.7217476858942</v>
@@ -38430,7 +38430,7 @@
     </row>
     <row r="127">
       <c r="A127" s="0" t="n">
-        <v>94.53018822123072</v>
+        <v>112.7085978704786</v>
       </c>
       <c r="B127" s="0" t="n">
         <v>112.7085978704784</v>
@@ -38732,7 +38732,7 @@
     </row>
     <row r="128">
       <c r="A128" s="0" t="n">
-        <v>93.70250394995536</v>
+        <v>113.7041650086281</v>
       </c>
       <c r="B128" s="0" t="n">
         <v>113.7041650086278</v>
@@ -39034,7 +39034,7 @@
     </row>
     <row r="129">
       <c r="A129" s="0" t="n">
-        <v>94.53018822123074</v>
+        <v>114.708526098129</v>
       </c>
       <c r="B129" s="0" t="n">
         <v>112.7085978704784</v>
@@ -39336,7 +39336,7 @@
     </row>
     <row r="130">
       <c r="A130" s="0" t="n">
-        <v>93.70250394995539</v>
+        <v>115.7217588168972</v>
       </c>
       <c r="B130" s="0" t="n">
         <v>113.7041650086279</v>
@@ -39638,7 +39638,7 @@
     </row>
     <row r="131">
       <c r="A131" s="0" t="n">
-        <v>92.8820666890352</v>
+        <v>116.7439415289859</v>
       </c>
       <c r="B131" s="0" t="n">
         <v>112.7085978704784</v>
@@ -39940,7 +39940,7 @@
     </row>
     <row r="132">
       <c r="A132" s="0" t="n">
-        <v>92.06881298533848</v>
+        <v>117.7751532906465</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>111.7217476858943</v>
@@ -40242,7 +40242,7 @@
     </row>
     <row r="133">
       <c r="A133" s="0" t="n">
-        <v>91.26267994131432</v>
+        <v>116.743941528986</v>
       </c>
       <c r="B133" s="0" t="n">
         <v>112.7085978704784</v>
@@ -40544,7 +40544,7 @@
     </row>
     <row r="134">
       <c r="A134" s="0" t="n">
-        <v>90.46360521012809</v>
+        <v>117.7751532906465</v>
       </c>
       <c r="B134" s="0" t="n">
         <v>113.7041650086279</v>
@@ -40846,7 +40846,7 @@
     </row>
     <row r="135">
       <c r="A135" s="0" t="n">
-        <v>91.26267994131433</v>
+        <v>116.743941528986</v>
       </c>
       <c r="B135" s="0" t="n">
         <v>112.7085978704784</v>
@@ -41148,7 +41148,7 @@
     </row>
     <row r="136">
       <c r="A136" s="0" t="n">
-        <v>92.06881298533851</v>
+        <v>117.7751532906465</v>
       </c>
       <c r="B136" s="0" t="n">
         <v>111.7217476858943</v>
@@ -41450,7 +41450,7 @@
     </row>
     <row r="137">
       <c r="A137" s="0" t="n">
-        <v>92.88206668903524</v>
+        <v>118.8154738564425</v>
       </c>
       <c r="B137" s="0" t="n">
         <v>110.743538131264</v>
@@ -41752,7 +41752,7 @@
     </row>
     <row r="138">
       <c r="A138" s="0" t="n">
-        <v>93.70250394995544</v>
+        <v>117.7751532906465</v>
       </c>
       <c r="B138" s="0" t="n">
         <v>109.7738935512477</v>
@@ -42054,7 +42054,7 @@
     </row>
     <row r="139">
       <c r="A139" s="0" t="n">
-        <v>92.88206668903526</v>
+        <v>116.743941528986</v>
       </c>
       <c r="B139" s="0" t="n">
         <v>108.8127389529263</v>
@@ -42356,7 +42356,7 @@
     </row>
     <row r="140">
       <c r="A140" s="0" t="n">
-        <v>93.70250394995546</v>
+        <v>115.7217588168973</v>
       </c>
       <c r="B140" s="0" t="n">
         <v>109.7738935512478</v>
@@ -42658,7 +42658,7 @@
     </row>
     <row r="141">
       <c r="A141" s="0" t="n">
-        <v>92.88206668903527</v>
+        <v>114.7085260981292</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>108.8127389529263</v>
@@ -42960,7 +42960,7 @@
     </row>
     <row r="142">
       <c r="A142" s="0" t="n">
-        <v>92.06881298533855</v>
+        <v>113.7041650086283</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>109.7738935512478</v>
@@ -43262,7 +43262,7 @@
     </row>
     <row r="143">
       <c r="A143" s="0" t="n">
-        <v>92.88206668903528</v>
+        <v>114.7085260981292</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>108.8127389529264</v>
@@ -43564,7 +43564,7 @@
     </row>
     <row r="144">
       <c r="A144" s="0" t="n">
-        <v>93.70250394995549</v>
+        <v>115.7217588168974</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>107.860000000001</v>
@@ -43866,7 +43866,7 @@
     </row>
     <row r="145">
       <c r="A145" s="0" t="n">
-        <v>92.8820666890353</v>
+        <v>116.7439415289861</v>
       </c>
       <c r="B145" s="0" t="n">
         <v>106.9156030070443</v>
@@ -44168,7 +44168,7 @@
     </row>
     <row r="146">
       <c r="A146" s="0" t="n">
-        <v>93.7025039499555</v>
+        <v>117.7751532906466</v>
       </c>
       <c r="B146" s="0" t="n">
         <v>105.9794749338012</v>
@@ -44470,7 +44470,7 @@
     </row>
     <row r="147">
       <c r="A147" s="0" t="n">
-        <v>92.88206668903531</v>
+        <v>116.7439415289862</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>106.9156030070443</v>
@@ -44772,7 +44772,7 @@
     </row>
     <row r="148">
       <c r="A148" s="0" t="n">
-        <v>92.0688129853386</v>
+        <v>115.7217588168975</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>105.9794749338012</v>
@@ -45074,7 +45074,7 @@
     </row>
     <row r="149">
       <c r="A149" s="0" t="n">
-        <v>91.26267994131443</v>
+        <v>114.7085260981293</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>105.05154337954</v>
@@ -45376,7 +45376,7 @@
     </row>
     <row r="150">
       <c r="A150" s="0" t="n">
-        <v>92.06881298533861</v>
+        <v>113.7041650086284</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>104.1317365774531</v>
@@ -45678,7 +45678,7 @@
     </row>
     <row r="151">
       <c r="A151" s="0" t="n">
-        <v>91.26267994131445</v>
+        <v>114.7085260981293</v>
       </c>
       <c r="B151" s="0" t="n">
         <v>103.2199833891061</v>
@@ -45980,7 +45980,7 @@
     </row>
     <row r="152">
       <c r="A152" s="0" t="n">
-        <v>90.46360521012821</v>
+        <v>113.7041650086284</v>
       </c>
       <c r="B152" s="0" t="n">
         <v>102.3162132989363</v>
@@ -46282,7 +46282,7 @@
     </row>
     <row r="153">
       <c r="A153" s="0" t="n">
-        <v>91.26267994131446</v>
+        <v>114.7085260981293</v>
       </c>
       <c r="B153" s="0" t="n">
         <v>103.2199833891061</v>
@@ -46584,7 +46584,7 @@
     </row>
     <row r="154">
       <c r="A154" s="0" t="n">
-        <v>92.06881298533864</v>
+        <v>113.7041650086284</v>
       </c>
       <c r="B154" s="0" t="n">
         <v>104.1317365774531</v>
@@ -46886,7 +46886,7 @@
     </row>
     <row r="155">
       <c r="A155" s="0" t="n">
-        <v>91.26267994131447</v>
+        <v>112.708597870479</v>
       </c>
       <c r="B155" s="0" t="n">
         <v>103.2199833891061</v>
@@ -47188,7 +47188,7 @@
     </row>
     <row r="156">
       <c r="A156" s="0" t="n">
-        <v>92.06881298533865</v>
+        <v>113.7041650086284</v>
       </c>
       <c r="B156" s="0" t="n">
         <v>102.3162132989363</v>
@@ -47490,7 +47490,7 @@
     </row>
     <row r="157">
       <c r="A157" s="0" t="n">
-        <v>92.88206668903538</v>
+        <v>112.708597870479</v>
       </c>
       <c r="B157" s="0" t="n">
         <v>101.4203564087988</v>
@@ -47792,7 +47792,7 @@
     </row>
     <row r="158">
       <c r="A158" s="0" t="n">
-        <v>92.06881298533867</v>
+        <v>113.7041650086285</v>
       </c>
       <c r="B158" s="0" t="n">
         <v>102.3162132989364</v>
@@ -48094,7 +48094,7 @@
     </row>
     <row r="159">
       <c r="A159" s="0" t="n">
-        <v>92.8820666890354</v>
+        <v>114.7085260981294</v>
       </c>
       <c r="B159" s="0" t="n">
         <v>101.4203564087989</v>
@@ -48396,7 +48396,7 @@
     </row>
     <row r="160">
       <c r="A160" s="0" t="n">
-        <v>92.06881298533868</v>
+        <v>113.7041650086285</v>
       </c>
       <c r="B160" s="0" t="n">
         <v>100.5323434325605</v>
@@ -48698,7 +48698,7 @@
     </row>
     <row r="161">
       <c r="A161" s="0" t="n">
-        <v>91.26267994131452</v>
+        <v>112.708597870479</v>
       </c>
       <c r="B161" s="0" t="n">
         <v>101.4203564087989</v>
@@ -49000,7 +49000,7 @@
     </row>
     <row r="162">
       <c r="A162" s="0" t="n">
-        <v>92.0688129853387</v>
+        <v>111.7217476858949</v>
       </c>
       <c r="B162" s="0" t="n">
         <v>100.5323434325605</v>
@@ -49302,7 +49302,7 @@
     </row>
     <row r="163">
       <c r="A163" s="0" t="n">
-        <v>91.26267994131453</v>
+        <v>110.7435381312646</v>
       </c>
       <c r="B163" s="0" t="n">
         <v>99.65210569074151</v>
@@ -49604,7 +49604,7 @@
     </row>
     <row r="164">
       <c r="A164" s="0" t="n">
-        <v>92.06881298533871</v>
+        <v>111.7217476858949</v>
       </c>
       <c r="B164" s="0" t="n">
         <v>100.5323434325606</v>
@@ -49906,7 +49906,7 @@
     </row>
     <row r="165">
       <c r="A165" s="0" t="n">
-        <v>92.88206668903545</v>
+        <v>110.7435381312646</v>
       </c>
       <c r="B165" s="0" t="n">
         <v>101.4203564087989</v>
@@ -50208,7 +50208,7 @@
     </row>
     <row r="166">
       <c r="A166" s="0" t="n">
-        <v>93.70250394995566</v>
+        <v>111.7217476858949</v>
       </c>
       <c r="B166" s="0" t="n">
         <v>100.5323434325606</v>
@@ -50510,7 +50510,7 @@
     </row>
     <row r="167">
       <c r="A167" s="0" t="n">
-        <v>92.88206668903547</v>
+        <v>112.7085978704791</v>
       </c>
       <c r="B167" s="0" t="n">
         <v>99.65210569074154</v>
@@ -50812,7 +50812,7 @@
     </row>
     <row r="168">
       <c r="A168" s="0" t="n">
-        <v>93.70250394995567</v>
+        <v>111.721747685895</v>
       </c>
       <c r="B168" s="0" t="n">
         <v>100.5323434325606</v>
@@ -51114,7 +51114,7 @@
     </row>
     <row r="169">
       <c r="A169" s="0" t="n">
-        <v>94.53018822123106</v>
+        <v>112.7085978704791</v>
       </c>
       <c r="B169" s="0" t="n">
         <v>99.65210569074155</v>
@@ -51416,7 +51416,7 @@
     </row>
     <row r="170">
       <c r="A170" s="0" t="n">
-        <v>93.70250394995568</v>
+        <v>113.7041650086286</v>
       </c>
       <c r="B170" s="0" t="n">
         <v>100.5323434325606</v>
@@ -51718,7 +51718,7 @@
     </row>
     <row r="171">
       <c r="A171" s="0" t="n">
-        <v>94.53018822123107</v>
+        <v>112.7085978704791</v>
       </c>
       <c r="B171" s="0" t="n">
         <v>99.65210569074156</v>
@@ -52020,7 +52020,7 @@
     </row>
     <row r="172">
       <c r="A172" s="0" t="n">
-        <v>95.36518351648168</v>
+        <v>111.721747685895</v>
       </c>
       <c r="B172" s="0" t="n">
         <v>98.77957510520346</v>
@@ -52322,7 +52322,7 @@
     </row>
     <row r="173">
       <c r="A173" s="0" t="n">
-        <v>94.53018822123109</v>
+        <v>110.7435381312647</v>
       </c>
       <c r="B173" s="0" t="n">
         <v>97.91468419388421</v>
@@ -52624,7 +52624,7 @@
     </row>
     <row r="174">
       <c r="A174" s="0" t="n">
-        <v>95.36518351648169</v>
+        <v>109.7738935512484</v>
       </c>
       <c r="B174" s="0" t="n">
         <v>97.05736606557892</v>
@@ -52926,7 +52926,7 @@
     </row>
     <row r="175">
       <c r="A175" s="0" t="n">
-        <v>96.20755441476675</v>
+        <v>110.7435381312647</v>
       </c>
       <c r="B175" s="0" t="n">
         <v>96.20755441476648</v>
@@ -53228,7 +53228,7 @@
     </row>
     <row r="176">
       <c r="A176" s="0" t="n">
-        <v>97.0573660655792</v>
+        <v>111.721747685895</v>
       </c>
       <c r="B176" s="0" t="n">
         <v>97.05736606557893</v>
@@ -53530,7 +53530,7 @@
     </row>
     <row r="177">
       <c r="A177" s="0" t="n">
-        <v>97.91468419388451</v>
+        <v>112.7085978704792</v>
       </c>
       <c r="B177" s="0" t="n">
         <v>97.91468419388424</v>
@@ -53832,7 +53832,7 @@
     </row>
     <row r="178">
       <c r="A178" s="0" t="n">
-        <v>98.77957510520378</v>
+        <v>113.7041650086287</v>
       </c>
       <c r="B178" s="0" t="n">
         <v>97.05736606557895</v>
@@ -54134,7 +54134,7 @@
     </row>
     <row r="179">
       <c r="A179" s="0" t="n">
-        <v>97.91468419388453</v>
+        <v>112.7085978704792</v>
       </c>
       <c r="B179" s="0" t="n">
         <v>96.20755441476651</v>
@@ -54436,7 +54436,7 @@
     </row>
     <row r="180">
       <c r="A180" s="0" t="n">
-        <v>97.05736606557923</v>
+        <v>111.7217476858951</v>
       </c>
       <c r="B180" s="0" t="n">
         <v>97.05736606557896</v>

</xml_diff>